<commit_message>
split evaluating and predicting
</commit_message>
<xml_diff>
--- a/notebook/results/Model-v1-Results.xlsx
+++ b/notebook/results/Model-v1-Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HAW\Bachelorarbeit\TranslationT5\notebook\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE4F216-B281-4361-A58C-728F21DD7D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564FE108-9358-4C24-8304-A08793979589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4392" yWindow="3456" windowWidth="17640" windowHeight="8904" xr2:uid="{5C25365D-9598-4416-8DEF-A2E75805290F}"/>
+    <workbookView xWindow="4272" yWindow="276" windowWidth="17640" windowHeight="8904" xr2:uid="{5C25365D-9598-4416-8DEF-A2E75805290F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -99,13 +99,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -123,11 +140,11 @@
   <autoFilter ref="A1:F5" xr:uid="{3097FC38-72C4-4A6B-9C80-5483D098EB6E}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E2818F8C-4597-484B-9D19-1491B90AA33A}" name="Decoding Method"/>
-    <tableColumn id="2" xr3:uid="{789937A5-F7BF-456C-BE1D-7E568A5D9F46}" name="F1-Score"/>
-    <tableColumn id="3" xr3:uid="{2E15D060-2087-4AFB-BE53-A0B75B5341E3}" name="Bleu 1 Translation"/>
-    <tableColumn id="4" xr3:uid="{13B94D85-B122-42DE-961E-FAB862A3218E}" name="Bleu 3 Translations"/>
-    <tableColumn id="5" xr3:uid="{E4AE71E0-F573-41F9-9ABB-8DEAACAC1CEB}" name="Bleu 1 WMT"/>
-    <tableColumn id="6" xr3:uid="{3481A0A0-E298-445D-B241-7269A9C35D99}" name="Bleu 3 WMT"/>
+    <tableColumn id="2" xr3:uid="{789937A5-F7BF-456C-BE1D-7E568A5D9F46}" name="F1-Score" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{2E15D060-2087-4AFB-BE53-A0B75B5341E3}" name="Bleu 1 Translation" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{13B94D85-B122-42DE-961E-FAB862A3218E}" name="Bleu 3 Translations" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{E4AE71E0-F573-41F9-9ABB-8DEAACAC1CEB}" name="Bleu 1 WMT" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{3481A0A0-E298-445D-B241-7269A9C35D99}" name="Bleu 3 WMT" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -433,7 +450,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,7 +459,8 @@
     <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -469,20 +487,80 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="1">
+        <v>0.34182366120735902</v>
+      </c>
+      <c r="C2" s="1">
+        <v>58.5817266068387</v>
+      </c>
+      <c r="D2" s="1">
+        <v>54.371892507957298</v>
+      </c>
+      <c r="E2" s="1">
+        <v>19.561407387726302</v>
+      </c>
+      <c r="F2" s="1">
+        <v>19.511078188773201</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" s="1">
+        <v>0.28147622203288197</v>
+      </c>
+      <c r="C3" s="1">
+        <v>57.2424796521845</v>
+      </c>
+      <c r="D3" s="1">
+        <v>48.4727810559828</v>
+      </c>
+      <c r="E3" s="1">
+        <v>18.353755153828999</v>
+      </c>
+      <c r="F3" s="1">
+        <v>17.279835598492699</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
+      <c r="B4" s="1">
+        <v>0.25959481207990098</v>
+      </c>
+      <c r="C4" s="1">
+        <v>48.467653289467698</v>
+      </c>
+      <c r="D4" s="1">
+        <v>49.078043567809303</v>
+      </c>
+      <c r="E4" s="1">
+        <v>14.607165790417501</v>
+      </c>
+      <c r="F4" s="1">
+        <v>14.5870804303157</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.283959733661522</v>
+      </c>
+      <c r="C5" s="1">
+        <v>53.443229036504299</v>
+      </c>
+      <c r="D5" s="1">
+        <v>52.246567667076</v>
+      </c>
+      <c r="E5" s="1">
+        <v>15.509973904627</v>
+      </c>
+      <c r="F5" s="1">
+        <v>15.538847615420099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>